<commit_message>
minor adjustments to Scenario1
</commit_message>
<xml_diff>
--- a/Scenariu1.xlsx
+++ b/Scenariu1.xlsx
@@ -380,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J154"/>
+  <dimension ref="A1:J156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="E160" sqref="E160"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="L155" sqref="L155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5477,308 +5477,290 @@
       </c>
     </row>
     <row r="142" spans="1:10">
-      <c r="A142">
-        <f t="shared" si="16"/>
+      <c r="A142" s="1">
         <v>141</v>
       </c>
-      <c r="B142">
-        <f t="shared" si="15"/>
+      <c r="B142" s="1">
         <v>8</v>
       </c>
-      <c r="C142">
-        <v>100</v>
-      </c>
-      <c r="D142">
-        <v>0</v>
-      </c>
-      <c r="E142">
-        <v>0</v>
-      </c>
-      <c r="F142">
-        <v>0</v>
-      </c>
-      <c r="G142">
-        <v>0</v>
-      </c>
-      <c r="H142">
-        <v>0</v>
-      </c>
-      <c r="I142">
-        <v>0</v>
-      </c>
-      <c r="J142">
+      <c r="C142" s="1">
+        <v>100</v>
+      </c>
+      <c r="D142" s="1">
+        <v>0</v>
+      </c>
+      <c r="E142" s="1">
+        <v>0</v>
+      </c>
+      <c r="F142" s="1">
+        <v>0</v>
+      </c>
+      <c r="G142" s="1">
+        <v>0</v>
+      </c>
+      <c r="H142" s="1">
+        <v>0</v>
+      </c>
+      <c r="I142" s="1">
+        <v>0</v>
+      </c>
+      <c r="J142" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:10">
-      <c r="A143">
-        <f t="shared" si="16"/>
+      <c r="A143" s="1">
         <v>142</v>
       </c>
-      <c r="B143">
-        <f t="shared" si="15"/>
+      <c r="B143" s="1">
         <v>7</v>
       </c>
-      <c r="C143">
-        <v>100</v>
-      </c>
-      <c r="D143">
-        <v>0</v>
-      </c>
-      <c r="E143">
-        <v>0</v>
-      </c>
-      <c r="F143">
-        <v>0</v>
-      </c>
-      <c r="G143">
-        <v>0</v>
-      </c>
-      <c r="H143">
-        <v>0</v>
-      </c>
-      <c r="I143">
-        <v>0</v>
-      </c>
-      <c r="J143">
+      <c r="C143" s="1">
+        <v>100</v>
+      </c>
+      <c r="D143" s="1">
+        <v>0</v>
+      </c>
+      <c r="E143" s="1">
+        <v>0</v>
+      </c>
+      <c r="F143" s="1">
+        <v>0</v>
+      </c>
+      <c r="G143" s="1">
+        <v>0</v>
+      </c>
+      <c r="H143" s="1">
+        <v>0</v>
+      </c>
+      <c r="I143" s="1">
+        <v>0</v>
+      </c>
+      <c r="J143" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:10">
-      <c r="A144">
-        <f t="shared" si="16"/>
+      <c r="A144" s="1">
         <v>143</v>
       </c>
-      <c r="B144">
-        <f t="shared" si="15"/>
+      <c r="B144" s="1">
         <v>6</v>
       </c>
-      <c r="C144">
-        <v>100</v>
-      </c>
-      <c r="D144">
-        <v>0</v>
-      </c>
-      <c r="E144">
-        <v>0</v>
-      </c>
-      <c r="F144">
-        <v>0</v>
-      </c>
-      <c r="G144">
-        <v>0</v>
-      </c>
-      <c r="H144">
-        <v>0</v>
-      </c>
-      <c r="I144">
-        <v>0</v>
-      </c>
-      <c r="J144">
+      <c r="C144" s="1">
+        <v>100</v>
+      </c>
+      <c r="D144" s="1">
+        <v>0</v>
+      </c>
+      <c r="E144" s="1">
+        <v>0</v>
+      </c>
+      <c r="F144" s="1">
+        <v>0</v>
+      </c>
+      <c r="G144" s="1">
+        <v>0</v>
+      </c>
+      <c r="H144" s="1">
+        <v>0</v>
+      </c>
+      <c r="I144" s="1">
+        <v>0</v>
+      </c>
+      <c r="J144" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:10">
-      <c r="A145">
-        <f t="shared" si="16"/>
+      <c r="A145" s="1">
         <v>144</v>
       </c>
-      <c r="B145">
-        <f>B144-1</f>
+      <c r="B145" s="1">
         <v>5</v>
       </c>
-      <c r="C145">
-        <v>100</v>
-      </c>
-      <c r="D145">
-        <v>0</v>
-      </c>
-      <c r="E145">
-        <v>0</v>
-      </c>
-      <c r="F145">
-        <v>0</v>
-      </c>
-      <c r="G145">
-        <v>0</v>
-      </c>
-      <c r="H145">
-        <v>0</v>
-      </c>
-      <c r="I145">
-        <v>0</v>
-      </c>
-      <c r="J145">
+      <c r="C145" s="1">
+        <v>100</v>
+      </c>
+      <c r="D145" s="1">
+        <v>0</v>
+      </c>
+      <c r="E145" s="1">
+        <v>0</v>
+      </c>
+      <c r="F145" s="1">
+        <v>0</v>
+      </c>
+      <c r="G145" s="1">
+        <v>0</v>
+      </c>
+      <c r="H145" s="1">
+        <v>0</v>
+      </c>
+      <c r="I145" s="1">
+        <v>0</v>
+      </c>
+      <c r="J145" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:10">
-      <c r="A146">
-        <f t="shared" si="16"/>
+      <c r="A146" s="1">
         <v>145</v>
       </c>
-      <c r="B146">
-        <f t="shared" si="15"/>
+      <c r="B146" s="1">
         <v>4</v>
       </c>
-      <c r="C146">
-        <v>100</v>
-      </c>
-      <c r="D146">
-        <v>0</v>
-      </c>
-      <c r="E146">
-        <v>0</v>
-      </c>
-      <c r="F146">
-        <v>0</v>
-      </c>
-      <c r="G146">
-        <v>0</v>
-      </c>
-      <c r="H146">
-        <v>0</v>
-      </c>
-      <c r="I146">
-        <v>0</v>
-      </c>
-      <c r="J146">
+      <c r="C146" s="1">
+        <v>100</v>
+      </c>
+      <c r="D146" s="1">
+        <v>0</v>
+      </c>
+      <c r="E146" s="1">
+        <v>0</v>
+      </c>
+      <c r="F146" s="1">
+        <v>0</v>
+      </c>
+      <c r="G146" s="1">
+        <v>0</v>
+      </c>
+      <c r="H146" s="1">
+        <v>0</v>
+      </c>
+      <c r="I146" s="1">
+        <v>0</v>
+      </c>
+      <c r="J146" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:10">
-      <c r="A147">
-        <f t="shared" si="16"/>
+      <c r="A147" s="1">
         <v>146</v>
       </c>
-      <c r="B147">
-        <f t="shared" si="15"/>
+      <c r="B147" s="1">
         <v>3</v>
       </c>
-      <c r="C147">
-        <v>100</v>
-      </c>
-      <c r="D147">
-        <v>0</v>
-      </c>
-      <c r="E147">
-        <v>0</v>
-      </c>
-      <c r="F147">
-        <v>0</v>
-      </c>
-      <c r="G147">
-        <v>0</v>
-      </c>
-      <c r="H147">
-        <v>0</v>
-      </c>
-      <c r="I147">
-        <v>0</v>
-      </c>
-      <c r="J147">
+      <c r="C147" s="1">
+        <v>100</v>
+      </c>
+      <c r="D147" s="1">
+        <v>0</v>
+      </c>
+      <c r="E147" s="1">
+        <v>0</v>
+      </c>
+      <c r="F147" s="1">
+        <v>0</v>
+      </c>
+      <c r="G147" s="1">
+        <v>0</v>
+      </c>
+      <c r="H147" s="1">
+        <v>0</v>
+      </c>
+      <c r="I147" s="1">
+        <v>0</v>
+      </c>
+      <c r="J147" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:10">
-      <c r="A148">
-        <f t="shared" si="16"/>
+      <c r="A148" s="1">
         <v>147</v>
       </c>
-      <c r="B148">
-        <f>B147-1</f>
+      <c r="B148" s="1">
         <v>2</v>
       </c>
-      <c r="C148">
-        <v>100</v>
-      </c>
-      <c r="D148">
-        <v>0</v>
-      </c>
-      <c r="E148">
-        <v>0</v>
-      </c>
-      <c r="F148">
-        <v>0</v>
-      </c>
-      <c r="G148">
-        <v>0</v>
-      </c>
-      <c r="H148">
-        <v>0</v>
-      </c>
-      <c r="I148">
-        <v>0</v>
-      </c>
-      <c r="J148">
+      <c r="C148" s="1">
+        <v>100</v>
+      </c>
+      <c r="D148" s="1">
+        <v>0</v>
+      </c>
+      <c r="E148" s="1">
+        <v>0</v>
+      </c>
+      <c r="F148" s="1">
+        <v>0</v>
+      </c>
+      <c r="G148" s="1">
+        <v>0</v>
+      </c>
+      <c r="H148" s="1">
+        <v>0</v>
+      </c>
+      <c r="I148" s="1">
+        <v>0</v>
+      </c>
+      <c r="J148" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:10">
-      <c r="A149">
-        <f t="shared" si="16"/>
+      <c r="A149" s="1">
         <v>148</v>
       </c>
-      <c r="B149">
-        <f t="shared" si="15"/>
+      <c r="B149" s="1">
         <v>1</v>
       </c>
-      <c r="C149">
-        <v>100</v>
-      </c>
-      <c r="D149">
-        <v>0</v>
-      </c>
-      <c r="E149">
-        <v>0</v>
-      </c>
-      <c r="F149">
-        <v>0</v>
-      </c>
-      <c r="G149">
-        <v>0</v>
-      </c>
-      <c r="H149">
-        <v>0</v>
-      </c>
-      <c r="I149">
-        <v>0</v>
-      </c>
-      <c r="J149">
+      <c r="C149" s="1">
+        <v>100</v>
+      </c>
+      <c r="D149" s="1">
+        <v>0</v>
+      </c>
+      <c r="E149" s="1">
+        <v>0</v>
+      </c>
+      <c r="F149" s="1">
+        <v>0</v>
+      </c>
+      <c r="G149" s="1">
+        <v>0</v>
+      </c>
+      <c r="H149" s="1">
+        <v>0</v>
+      </c>
+      <c r="I149" s="1">
+        <v>0</v>
+      </c>
+      <c r="J149" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:10">
-      <c r="A150">
-        <f t="shared" si="16"/>
+      <c r="A150" s="1">
         <v>149</v>
       </c>
-      <c r="B150">
-        <f>B149-1</f>
-        <v>0</v>
-      </c>
-      <c r="C150">
+      <c r="B150" s="1">
+        <v>0</v>
+      </c>
+      <c r="C150" s="1">
         <v>5000</v>
       </c>
-      <c r="D150">
-        <v>0</v>
-      </c>
-      <c r="E150">
-        <v>0</v>
-      </c>
-      <c r="F150">
-        <v>0</v>
-      </c>
-      <c r="G150">
-        <v>0</v>
-      </c>
-      <c r="H150">
-        <v>0</v>
-      </c>
-      <c r="I150">
-        <v>0</v>
-      </c>
-      <c r="J150">
+      <c r="D150" s="1">
+        <v>0</v>
+      </c>
+      <c r="E150" s="1">
+        <v>0</v>
+      </c>
+      <c r="F150" s="1">
+        <v>0</v>
+      </c>
+      <c r="G150" s="1">
+        <v>0</v>
+      </c>
+      <c r="H150" s="1">
+        <v>0</v>
+      </c>
+      <c r="I150" s="1">
+        <v>0</v>
+      </c>
+      <c r="J150" s="1">
         <v>0</v>
       </c>
     </row>
@@ -5898,15 +5880,79 @@
         <v>0</v>
       </c>
       <c r="G154" s="1">
+        <v>0</v>
+      </c>
+      <c r="H154" s="1">
+        <v>0</v>
+      </c>
+      <c r="I154" s="1">
+        <v>0</v>
+      </c>
+      <c r="J154" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10">
+      <c r="A155" s="1">
+        <v>154</v>
+      </c>
+      <c r="B155" s="1">
+        <v>0</v>
+      </c>
+      <c r="C155" s="1">
+        <v>100</v>
+      </c>
+      <c r="D155" s="1">
+        <v>0</v>
+      </c>
+      <c r="E155" s="1">
+        <v>0</v>
+      </c>
+      <c r="F155" s="1">
+        <v>0</v>
+      </c>
+      <c r="G155" s="1">
         <v>1</v>
       </c>
-      <c r="H154" s="1">
-        <v>0</v>
-      </c>
-      <c r="I154" s="1">
-        <v>0</v>
-      </c>
-      <c r="J154" s="1">
+      <c r="H155" s="1">
+        <v>0</v>
+      </c>
+      <c r="I155" s="1">
+        <v>0</v>
+      </c>
+      <c r="J155" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10">
+      <c r="A156" s="1">
+        <v>155</v>
+      </c>
+      <c r="B156" s="1">
+        <v>0</v>
+      </c>
+      <c r="C156" s="1">
+        <v>100</v>
+      </c>
+      <c r="D156" s="1">
+        <v>0</v>
+      </c>
+      <c r="E156" s="1">
+        <v>0</v>
+      </c>
+      <c r="F156" s="1">
+        <v>0</v>
+      </c>
+      <c r="G156" s="1">
+        <v>0</v>
+      </c>
+      <c r="H156" s="1">
+        <v>0</v>
+      </c>
+      <c r="I156" s="1">
+        <v>0</v>
+      </c>
+      <c r="J156" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implemented second scenario and 3 small test scenarios
</commit_message>
<xml_diff>
--- a/Scenariu1.xlsx
+++ b/Scenariu1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="15135" windowHeight="8130"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ID</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>DECELERARE</t>
+  </si>
+  <si>
+    <t>BRAKE</t>
   </si>
 </sst>
 </file>
@@ -380,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J156"/>
+  <dimension ref="A1:K156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="L155" sqref="L155"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -391,7 +394,7 @@
     <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,8 +425,11 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
@@ -454,8 +460,11 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -492,8 +501,11 @@
       <c r="J3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
         <f t="shared" ref="A4" si="0">A3+1</f>
         <v>3</v>
@@ -513,8 +525,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
@@ -530,8 +541,11 @@
       <c r="J4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
         <f>A4+1</f>
         <v>4</v>
@@ -563,8 +577,11 @@
       <c r="J5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <f t="shared" ref="A6:A69" si="2">A5+1</f>
         <v>5</v>
@@ -585,8 +602,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <f>F4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f>G4</f>
@@ -602,8 +618,11 @@
       <c r="J6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -625,7 +644,6 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G7">
@@ -642,8 +660,11 @@
       <c r="J7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -682,8 +703,11 @@
       <c r="J8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -722,8 +746,11 @@
       <c r="J9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -762,8 +789,11 @@
       <c r="J10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -802,8 +832,11 @@
       <c r="J11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -842,8 +875,11 @@
       <c r="J12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -882,8 +918,11 @@
       <c r="J13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -922,8 +961,11 @@
       <c r="J14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -962,8 +1004,11 @@
       <c r="J15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -1002,8 +1047,11 @@
       <c r="J16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -1042,8 +1090,11 @@
       <c r="J17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -1082,8 +1133,11 @@
       <c r="J18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -1122,8 +1176,11 @@
       <c r="J19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -1162,8 +1219,11 @@
       <c r="J20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -1202,8 +1262,11 @@
       <c r="J21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -1242,8 +1305,11 @@
       <c r="J22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -1282,8 +1348,11 @@
       <c r="J23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -1322,8 +1391,11 @@
       <c r="J24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -1362,8 +1434,11 @@
       <c r="J25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -1402,8 +1477,11 @@
       <c r="J26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -1442,8 +1520,11 @@
       <c r="J27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -1482,8 +1563,11 @@
       <c r="J28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="K28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -1522,8 +1606,11 @@
       <c r="J29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -1562,8 +1649,11 @@
       <c r="J30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="K30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -1602,8 +1692,11 @@
       <c r="J31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -1642,8 +1735,11 @@
       <c r="J32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="K32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -1682,8 +1778,11 @@
       <c r="J33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="K33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -1722,8 +1821,11 @@
       <c r="J34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="K34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -1762,8 +1864,11 @@
       <c r="J35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="K35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -1802,8 +1907,11 @@
       <c r="J36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="K36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -1842,8 +1950,11 @@
       <c r="J37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="K37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -1882,8 +1993,11 @@
       <c r="J38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="K38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -1922,8 +2036,11 @@
       <c r="J39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="K39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -1962,8 +2079,11 @@
       <c r="J40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="K40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -2002,8 +2122,11 @@
       <c r="J41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:10">
+      <c r="K41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -2042,8 +2165,11 @@
       <c r="J42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:10">
+      <c r="K42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -2082,8 +2208,11 @@
       <c r="J43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:10">
+      <c r="K43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -2122,8 +2251,11 @@
       <c r="J44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:10">
+      <c r="K44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -2162,8 +2294,11 @@
       <c r="J45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="K45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -2202,8 +2337,11 @@
       <c r="J46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:10">
+      <c r="K46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -2242,8 +2380,11 @@
       <c r="J47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:10">
+      <c r="K47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -2282,8 +2423,11 @@
       <c r="J48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:10">
+      <c r="K48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -2322,8 +2466,11 @@
       <c r="J49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:10">
+      <c r="K49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -2362,8 +2509,11 @@
       <c r="J50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:10">
+      <c r="K50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -2402,8 +2552,11 @@
       <c r="J51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:10">
+      <c r="K51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52">
         <f t="shared" si="2"/>
         <v>51</v>
@@ -2442,8 +2595,11 @@
       <c r="J52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:10">
+      <c r="K52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53">
         <f t="shared" si="2"/>
         <v>52</v>
@@ -2482,8 +2638,11 @@
       <c r="J53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:10">
+      <c r="K53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54">
         <f t="shared" si="2"/>
         <v>53</v>
@@ -2522,8 +2681,11 @@
       <c r="J54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:10">
+      <c r="K54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55">
         <f t="shared" si="2"/>
         <v>54</v>
@@ -2556,8 +2718,11 @@
       <c r="J55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:10">
+      <c r="K55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56">
         <f t="shared" si="2"/>
         <v>55</v>
@@ -2589,8 +2754,11 @@
       <c r="J56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:10">
+      <c r="K56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57">
         <f t="shared" si="2"/>
         <v>56</v>
@@ -2623,8 +2791,11 @@
       <c r="J57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:10">
+      <c r="K57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58">
         <f t="shared" si="2"/>
         <v>57</v>
@@ -2657,8 +2828,11 @@
       <c r="J58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:10">
+      <c r="K58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59">
         <f t="shared" si="2"/>
         <v>58</v>
@@ -2691,8 +2865,11 @@
       <c r="J59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:10">
+      <c r="K59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60">
         <f t="shared" si="2"/>
         <v>59</v>
@@ -2725,8 +2902,11 @@
       <c r="J60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:10">
+      <c r="K60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61">
         <f t="shared" si="2"/>
         <v>60</v>
@@ -2759,8 +2939,11 @@
       <c r="J61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:10">
+      <c r="K61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62">
         <f t="shared" si="2"/>
         <v>61</v>
@@ -2793,8 +2976,11 @@
       <c r="J62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:10">
+      <c r="K62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="A63">
         <f t="shared" si="2"/>
         <v>62</v>
@@ -2827,8 +3013,11 @@
       <c r="J63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:10">
+      <c r="K63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
       <c r="A64">
         <f t="shared" si="2"/>
         <v>63</v>
@@ -2861,8 +3050,11 @@
       <c r="J64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:10">
+      <c r="K64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65">
         <f t="shared" si="2"/>
         <v>64</v>
@@ -2895,8 +3087,11 @@
       <c r="J65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:10">
+      <c r="K65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66">
         <f t="shared" si="2"/>
         <v>65</v>
@@ -2929,8 +3124,11 @@
       <c r="J66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:10">
+      <c r="K66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67">
         <f t="shared" si="2"/>
         <v>66</v>
@@ -2963,8 +3161,11 @@
       <c r="J67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:10">
+      <c r="K67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
       <c r="A68">
         <f t="shared" si="2"/>
         <v>67</v>
@@ -2997,8 +3198,11 @@
       <c r="J68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:10">
+      <c r="K68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69">
         <f t="shared" si="2"/>
         <v>68</v>
@@ -3031,8 +3235,11 @@
       <c r="J69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:10">
+      <c r="K69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70">
         <f t="shared" ref="A70:A133" si="13">A69+1</f>
         <v>69</v>
@@ -3065,8 +3272,11 @@
       <c r="J70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:10">
+      <c r="K70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
       <c r="A71">
         <f t="shared" si="13"/>
         <v>70</v>
@@ -3099,8 +3309,11 @@
       <c r="J71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:10">
+      <c r="K71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
       <c r="A72">
         <f t="shared" si="13"/>
         <v>71</v>
@@ -3133,8 +3346,11 @@
       <c r="J72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:10">
+      <c r="K72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73">
         <f t="shared" si="13"/>
         <v>72</v>
@@ -3167,8 +3383,11 @@
       <c r="J73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:10">
+      <c r="K73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74">
         <f t="shared" si="13"/>
         <v>73</v>
@@ -3201,8 +3420,11 @@
       <c r="J74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:10">
+      <c r="K74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
       <c r="A75">
         <f t="shared" si="13"/>
         <v>74</v>
@@ -3235,8 +3457,11 @@
       <c r="J75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:10">
+      <c r="K75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
       <c r="A76">
         <f t="shared" si="13"/>
         <v>75</v>
@@ -3269,8 +3494,11 @@
       <c r="J76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:10">
+      <c r="K76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77">
         <f t="shared" si="13"/>
         <v>76</v>
@@ -3302,8 +3530,11 @@
       <c r="J77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:10">
+      <c r="K77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78">
         <f t="shared" si="13"/>
         <v>77</v>
@@ -3336,8 +3567,11 @@
       <c r="J78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:10">
+      <c r="K78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="A79">
         <f t="shared" si="13"/>
         <v>78</v>
@@ -3370,8 +3604,11 @@
       <c r="J79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:10">
+      <c r="K79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
       <c r="A80">
         <f t="shared" si="13"/>
         <v>79</v>
@@ -3404,8 +3641,11 @@
       <c r="J80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:10">
+      <c r="K80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
       <c r="A81">
         <f t="shared" si="13"/>
         <v>80</v>
@@ -3438,8 +3678,11 @@
       <c r="J81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:10">
+      <c r="K81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
       <c r="A82">
         <f t="shared" si="13"/>
         <v>81</v>
@@ -3472,8 +3715,11 @@
       <c r="J82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:10">
+      <c r="K82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
       <c r="A83">
         <f t="shared" si="13"/>
         <v>82</v>
@@ -3506,8 +3752,11 @@
       <c r="J83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:10">
+      <c r="K83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
       <c r="A84">
         <f t="shared" si="13"/>
         <v>83</v>
@@ -3540,8 +3789,11 @@
       <c r="J84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:10">
+      <c r="K84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
       <c r="A85">
         <f t="shared" si="13"/>
         <v>84</v>
@@ -3574,8 +3826,11 @@
       <c r="J85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:10">
+      <c r="K85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
       <c r="A86">
         <f t="shared" si="13"/>
         <v>85</v>
@@ -3608,8 +3863,11 @@
       <c r="J86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:10">
+      <c r="K86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
       <c r="A87">
         <f t="shared" si="13"/>
         <v>86</v>
@@ -3642,8 +3900,11 @@
       <c r="J87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:10">
+      <c r="K87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
       <c r="A88">
         <f t="shared" si="13"/>
         <v>87</v>
@@ -3676,8 +3937,11 @@
       <c r="J88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:10">
+      <c r="K88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
       <c r="A89">
         <f t="shared" si="13"/>
         <v>88</v>
@@ -3710,8 +3974,11 @@
       <c r="J89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:10">
+      <c r="K89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
       <c r="A90">
         <f t="shared" si="13"/>
         <v>89</v>
@@ -3744,8 +4011,11 @@
       <c r="J90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:10">
+      <c r="K90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
       <c r="A91">
         <f t="shared" si="13"/>
         <v>90</v>
@@ -3778,8 +4048,11 @@
       <c r="J91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:10">
+      <c r="K91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
       <c r="A92">
         <f t="shared" si="13"/>
         <v>91</v>
@@ -3812,8 +4085,11 @@
       <c r="J92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:10">
+      <c r="K92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
       <c r="A93">
         <f t="shared" si="13"/>
         <v>92</v>
@@ -3846,8 +4122,11 @@
       <c r="J93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:10">
+      <c r="K93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
       <c r="A94">
         <f t="shared" si="13"/>
         <v>93</v>
@@ -3880,8 +4159,11 @@
       <c r="J94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:10">
+      <c r="K94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
       <c r="A95">
         <f t="shared" si="13"/>
         <v>94</v>
@@ -3914,8 +4196,11 @@
       <c r="J95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:10">
+      <c r="K95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
       <c r="A96">
         <f t="shared" si="13"/>
         <v>95</v>
@@ -3948,8 +4233,11 @@
       <c r="J96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:10">
+      <c r="K96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
       <c r="A97">
         <f t="shared" si="13"/>
         <v>96</v>
@@ -3982,8 +4270,11 @@
       <c r="J97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:10">
+      <c r="K97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
       <c r="A98">
         <f t="shared" si="13"/>
         <v>97</v>
@@ -4016,8 +4307,11 @@
       <c r="J98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:10">
+      <c r="K98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
       <c r="A99">
         <f t="shared" si="13"/>
         <v>98</v>
@@ -4050,8 +4344,11 @@
       <c r="J99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:10">
+      <c r="K99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
       <c r="A100">
         <f t="shared" si="13"/>
         <v>99</v>
@@ -4084,8 +4381,11 @@
       <c r="J100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:10">
+      <c r="K100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
       <c r="A101">
         <f t="shared" si="13"/>
         <v>100</v>
@@ -4118,8 +4418,11 @@
       <c r="J101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:10">
+      <c r="K101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
       <c r="A102">
         <f t="shared" si="13"/>
         <v>101</v>
@@ -4152,8 +4455,11 @@
       <c r="J102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:10">
+      <c r="K102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
       <c r="A103">
         <f t="shared" si="13"/>
         <v>102</v>
@@ -4186,8 +4492,11 @@
       <c r="J103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:10">
+      <c r="K103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
       <c r="A104">
         <f t="shared" si="13"/>
         <v>103</v>
@@ -4220,8 +4529,11 @@
       <c r="J104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:10">
+      <c r="K104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
       <c r="A105">
         <f t="shared" si="13"/>
         <v>104</v>
@@ -4254,8 +4566,11 @@
       <c r="J105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:10">
+      <c r="K105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11">
       <c r="A106">
         <f t="shared" si="13"/>
         <v>105</v>
@@ -4288,8 +4603,11 @@
       <c r="J106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:10">
+      <c r="K106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11">
       <c r="A107">
         <f t="shared" si="13"/>
         <v>106</v>
@@ -4322,8 +4640,11 @@
       <c r="J107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:10">
+      <c r="K107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11">
       <c r="A108">
         <f t="shared" si="13"/>
         <v>107</v>
@@ -4356,8 +4677,11 @@
       <c r="J108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:10">
+      <c r="K108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11">
       <c r="A109">
         <f t="shared" si="13"/>
         <v>108</v>
@@ -4390,8 +4714,11 @@
       <c r="J109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:10">
+      <c r="K109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11">
       <c r="A110">
         <f t="shared" si="13"/>
         <v>109</v>
@@ -4424,8 +4751,11 @@
       <c r="J110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:10">
+      <c r="K110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11">
       <c r="A111">
         <f t="shared" si="13"/>
         <v>110</v>
@@ -4458,8 +4788,11 @@
       <c r="J111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:10">
+      <c r="K111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11">
       <c r="A112">
         <f t="shared" si="13"/>
         <v>111</v>
@@ -4492,8 +4825,11 @@
       <c r="J112">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:10">
+      <c r="K112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11">
       <c r="A113">
         <f t="shared" si="13"/>
         <v>112</v>
@@ -4526,8 +4862,11 @@
       <c r="J113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:10">
+      <c r="K113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11">
       <c r="A114">
         <f t="shared" si="13"/>
         <v>113</v>
@@ -4560,8 +4899,11 @@
       <c r="J114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:10">
+      <c r="K114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11">
       <c r="A115">
         <f t="shared" si="13"/>
         <v>114</v>
@@ -4594,8 +4936,11 @@
       <c r="J115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:10">
+      <c r="K115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11">
       <c r="A116">
         <f t="shared" si="13"/>
         <v>115</v>
@@ -4628,8 +4973,11 @@
       <c r="J116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:10">
+      <c r="K116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
       <c r="A117">
         <f t="shared" si="13"/>
         <v>116</v>
@@ -4662,8 +5010,11 @@
       <c r="J117">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:10">
+      <c r="K117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11">
       <c r="A118">
         <f t="shared" si="13"/>
         <v>117</v>
@@ -4696,8 +5047,11 @@
       <c r="J118">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:10">
+      <c r="K118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11">
       <c r="A119">
         <f t="shared" si="13"/>
         <v>118</v>
@@ -4730,8 +5084,11 @@
       <c r="J119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:10">
+      <c r="K119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11">
       <c r="A120">
         <f t="shared" si="13"/>
         <v>119</v>
@@ -4764,8 +5121,11 @@
       <c r="J120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:10">
+      <c r="K120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11">
       <c r="A121">
         <f t="shared" si="13"/>
         <v>120</v>
@@ -4798,8 +5158,11 @@
       <c r="J121">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:10">
+      <c r="K121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
       <c r="A122">
         <f t="shared" si="13"/>
         <v>121</v>
@@ -4832,8 +5195,11 @@
       <c r="J122">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:10">
+      <c r="K122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
       <c r="A123">
         <f t="shared" si="13"/>
         <v>122</v>
@@ -4866,8 +5232,11 @@
       <c r="J123">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:10">
+      <c r="K123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
       <c r="A124">
         <f t="shared" si="13"/>
         <v>123</v>
@@ -4900,8 +5269,11 @@
       <c r="J124">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:10">
+      <c r="K124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11">
       <c r="A125">
         <f t="shared" si="13"/>
         <v>124</v>
@@ -4934,8 +5306,11 @@
       <c r="J125">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:10">
+      <c r="K125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
       <c r="A126">
         <f t="shared" si="13"/>
         <v>125</v>
@@ -4968,8 +5343,11 @@
       <c r="J126">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:10">
+      <c r="K126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11">
       <c r="A127">
         <f t="shared" si="13"/>
         <v>126</v>
@@ -5002,8 +5380,11 @@
       <c r="J127">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:10">
+      <c r="K127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11">
       <c r="A128">
         <f t="shared" si="13"/>
         <v>127</v>
@@ -5035,8 +5416,11 @@
       <c r="J128">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:10">
+      <c r="K128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11">
       <c r="A129">
         <f t="shared" si="13"/>
         <v>128</v>
@@ -5068,8 +5452,11 @@
       <c r="J129">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:10">
+      <c r="K129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11">
       <c r="A130">
         <f t="shared" si="13"/>
         <v>129</v>
@@ -5101,8 +5488,11 @@
       <c r="J130">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:10">
+      <c r="K130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11">
       <c r="A131">
         <f t="shared" si="13"/>
         <v>130</v>
@@ -5135,14 +5525,17 @@
       <c r="J131">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:10">
+      <c r="K131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11">
       <c r="A132">
         <f t="shared" si="13"/>
         <v>131</v>
       </c>
       <c r="B132">
-        <f t="shared" ref="B132:B149" si="15">B131-1</f>
+        <f t="shared" ref="B132:B141" si="15">B131-1</f>
         <v>18</v>
       </c>
       <c r="C132">
@@ -5169,8 +5562,11 @@
       <c r="J132">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:10">
+      <c r="K132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11">
       <c r="A133">
         <f t="shared" si="13"/>
         <v>132</v>
@@ -5203,10 +5599,13 @@
       <c r="J133">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:10">
+      <c r="K133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11">
       <c r="A134">
-        <f t="shared" ref="A134:A150" si="16">A133+1</f>
+        <f t="shared" ref="A134:A141" si="16">A133+1</f>
         <v>133</v>
       </c>
       <c r="B134">
@@ -5237,8 +5636,11 @@
       <c r="J134">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:10">
+      <c r="K134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11">
       <c r="A135">
         <f t="shared" si="16"/>
         <v>134</v>
@@ -5271,8 +5673,11 @@
       <c r="J135">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:10">
+      <c r="K135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11">
       <c r="A136">
         <f t="shared" si="16"/>
         <v>135</v>
@@ -5305,8 +5710,11 @@
       <c r="J136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:10">
+      <c r="K136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11">
       <c r="A137">
         <f t="shared" si="16"/>
         <v>136</v>
@@ -5339,8 +5747,11 @@
       <c r="J137">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:10">
+      <c r="K137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11">
       <c r="A138">
         <f t="shared" si="16"/>
         <v>137</v>
@@ -5373,8 +5784,11 @@
       <c r="J138">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:10">
+      <c r="K138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11">
       <c r="A139">
         <f t="shared" si="16"/>
         <v>138</v>
@@ -5407,8 +5821,11 @@
       <c r="J139">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:10">
+      <c r="K139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11">
       <c r="A140">
         <f t="shared" si="16"/>
         <v>139</v>
@@ -5441,8 +5858,11 @@
       <c r="J140">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:10">
+      <c r="K140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11">
       <c r="A141">
         <f t="shared" si="16"/>
         <v>140</v>
@@ -5475,8 +5895,11 @@
       <c r="J141">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:10">
+      <c r="K141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -5507,8 +5930,11 @@
       <c r="J142" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:10">
+      <c r="K142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -5539,8 +5965,11 @@
       <c r="J143" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:10">
+      <c r="K143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -5571,8 +6000,11 @@
       <c r="J144" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:10">
+      <c r="K144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -5603,8 +6035,11 @@
       <c r="J145" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:10">
+      <c r="K145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -5635,8 +6070,11 @@
       <c r="J146" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:10">
+      <c r="K146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -5667,8 +6105,11 @@
       <c r="J147" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:10">
+      <c r="K147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -5699,8 +6140,11 @@
       <c r="J148" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:10">
+      <c r="K148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -5731,8 +6175,11 @@
       <c r="J149" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:10">
+      <c r="K149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -5763,8 +6210,11 @@
       <c r="J150" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:10">
+      <c r="K150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -5795,8 +6245,11 @@
       <c r="J151" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:10">
+      <c r="K151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -5827,8 +6280,11 @@
       <c r="J152" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:10">
+      <c r="K152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -5859,8 +6315,11 @@
       <c r="J153" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:10">
+      <c r="K153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -5891,8 +6350,11 @@
       <c r="J154" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="1:10">
+      <c r="K154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -5923,8 +6385,11 @@
       <c r="J155" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="1:10">
+      <c r="K155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -5953,6 +6418,9 @@
         <v>0</v>
       </c>
       <c r="J156" s="1">
+        <v>0</v>
+      </c>
+      <c r="K156">
         <v>0</v>
       </c>
     </row>

</xml_diff>